<commit_message>
Add screen to readme
</commit_message>
<xml_diff>
--- a/samples/sample.xlsx
+++ b/samples/sample.xlsx
@@ -366,40 +366,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -416,31 +416,31 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -475,10 +475,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -487,35 +483,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -599,35 +579,41 @@
   <dimension ref="A1:AMJ27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="I5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="8.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="19.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="5.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="7" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="17" style="7" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="18.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="21" style="8" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="23" style="8" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="7.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="7.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="7.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="6" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="7.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="7" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="7" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="7" width="6.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="996" min="25" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="997" style="8" width="9.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,34 +718,34 @@
       <c r="X2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="ALI2" s="0"/>
-      <c r="ALJ2" s="0"/>
-      <c r="ALK2" s="0"/>
-      <c r="ALL2" s="0"/>
-      <c r="ALM2" s="0"/>
-      <c r="ALN2" s="0"/>
-      <c r="ALO2" s="0"/>
-      <c r="ALP2" s="0"/>
-      <c r="ALQ2" s="0"/>
-      <c r="ALR2" s="0"/>
-      <c r="ALS2" s="0"/>
-      <c r="ALT2" s="0"/>
-      <c r="ALU2" s="0"/>
-      <c r="ALV2" s="0"/>
-      <c r="ALW2" s="0"/>
-      <c r="ALX2" s="0"/>
-      <c r="ALY2" s="0"/>
-      <c r="ALZ2" s="0"/>
-      <c r="AMA2" s="0"/>
-      <c r="AMB2" s="0"/>
-      <c r="AMC2" s="0"/>
-      <c r="AMD2" s="0"/>
-      <c r="AME2" s="0"/>
-      <c r="AMF2" s="0"/>
-      <c r="AMG2" s="0"/>
-      <c r="AMH2" s="0"/>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
+      <c r="ALI2" s="8"/>
+      <c r="ALJ2" s="8"/>
+      <c r="ALK2" s="8"/>
+      <c r="ALL2" s="8"/>
+      <c r="ALM2" s="8"/>
+      <c r="ALN2" s="8"/>
+      <c r="ALO2" s="8"/>
+      <c r="ALP2" s="8"/>
+      <c r="ALQ2" s="8"/>
+      <c r="ALR2" s="8"/>
+      <c r="ALS2" s="8"/>
+      <c r="ALT2" s="8"/>
+      <c r="ALU2" s="8"/>
+      <c r="ALV2" s="8"/>
+      <c r="ALW2" s="8"/>
+      <c r="ALX2" s="8"/>
+      <c r="ALY2" s="8"/>
+      <c r="ALZ2" s="8"/>
+      <c r="AMA2" s="8"/>
+      <c r="AMB2" s="8"/>
+      <c r="AMC2" s="8"/>
+      <c r="AMD2" s="8"/>
+      <c r="AME2" s="8"/>
+      <c r="AMF2" s="8"/>
+      <c r="AMG2" s="8"/>
+      <c r="AMH2" s="8"/>
+      <c r="AMI2" s="8"/>
+      <c r="AMJ2" s="8"/>
     </row>
     <row r="3" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
@@ -835,43 +821,43 @@
         <f aca="false">SUM(U3,W3)</f>
         <v>2</v>
       </c>
-      <c r="ALI3" s="0"/>
-      <c r="ALJ3" s="0"/>
-      <c r="ALK3" s="0"/>
-      <c r="ALL3" s="0"/>
-      <c r="ALM3" s="0"/>
-      <c r="ALN3" s="0"/>
-      <c r="ALO3" s="0"/>
-      <c r="ALP3" s="0"/>
-      <c r="ALQ3" s="0"/>
-      <c r="ALR3" s="0"/>
-      <c r="ALS3" s="0"/>
-      <c r="ALT3" s="0"/>
-      <c r="ALU3" s="0"/>
-      <c r="ALV3" s="0"/>
-      <c r="ALW3" s="0"/>
-      <c r="ALX3" s="0"/>
-      <c r="ALY3" s="0"/>
-      <c r="ALZ3" s="0"/>
-      <c r="AMA3" s="0"/>
-      <c r="AMB3" s="0"/>
-      <c r="AMC3" s="0"/>
-      <c r="AMD3" s="0"/>
-      <c r="AME3" s="0"/>
-      <c r="AMF3" s="0"/>
-      <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
+      <c r="ALI3" s="8"/>
+      <c r="ALJ3" s="8"/>
+      <c r="ALK3" s="8"/>
+      <c r="ALL3" s="8"/>
+      <c r="ALM3" s="8"/>
+      <c r="ALN3" s="8"/>
+      <c r="ALO3" s="8"/>
+      <c r="ALP3" s="8"/>
+      <c r="ALQ3" s="8"/>
+      <c r="ALR3" s="8"/>
+      <c r="ALS3" s="8"/>
+      <c r="ALT3" s="8"/>
+      <c r="ALU3" s="8"/>
+      <c r="ALV3" s="8"/>
+      <c r="ALW3" s="8"/>
+      <c r="ALX3" s="8"/>
+      <c r="ALY3" s="8"/>
+      <c r="ALZ3" s="8"/>
+      <c r="AMA3" s="8"/>
+      <c r="AMB3" s="8"/>
+      <c r="AMC3" s="8"/>
+      <c r="AMD3" s="8"/>
+      <c r="AME3" s="8"/>
+      <c r="AMF3" s="8"/>
+      <c r="AMG3" s="8"/>
+      <c r="AMH3" s="8"/>
+      <c r="AMI3" s="8"/>
+      <c r="AMJ3" s="8"/>
     </row>
     <row r="4" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="26" t="s">
@@ -880,22 +866,22 @@
       <c r="E4" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="28" t="s">
         <v>35</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="30" t="n">
+      <c r="I4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="J4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="30" t="n">
+      <c r="K4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="23" t="n">
@@ -908,13 +894,13 @@
       <c r="N4" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="31" t="n">
+      <c r="O4" s="6" t="n">
         <v>4</v>
       </c>
       <c r="P4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="31" t="n">
+      <c r="Q4" s="6" t="n">
         <v>3</v>
       </c>
       <c r="R4" s="24" t="n">
@@ -927,94 +913,92 @@
       <c r="T4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="U4" s="32" t="n">
+      <c r="U4" s="7" t="n">
         <v>1</v>
       </c>
       <c r="V4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="W4" s="32" t="n">
+      <c r="W4" s="7" t="n">
         <v>0</v>
       </c>
       <c r="X4" s="25" t="n">
         <f aca="false">SUM(U4,W4)</f>
         <v>1</v>
       </c>
-      <c r="ALI4" s="0"/>
-      <c r="ALJ4" s="0"/>
-      <c r="ALK4" s="0"/>
-      <c r="ALL4" s="0"/>
-      <c r="ALM4" s="0"/>
-      <c r="ALN4" s="0"/>
-      <c r="ALO4" s="0"/>
-      <c r="ALP4" s="0"/>
-      <c r="ALQ4" s="0"/>
-      <c r="ALR4" s="0"/>
-      <c r="ALS4" s="0"/>
-      <c r="ALT4" s="0"/>
-      <c r="ALU4" s="0"/>
-      <c r="ALV4" s="0"/>
-      <c r="ALW4" s="0"/>
-      <c r="ALX4" s="0"/>
-      <c r="ALY4" s="0"/>
-      <c r="ALZ4" s="0"/>
-      <c r="AMA4" s="0"/>
-      <c r="AMB4" s="0"/>
-      <c r="AMC4" s="0"/>
-      <c r="AMD4" s="0"/>
-      <c r="AME4" s="0"/>
-      <c r="AMF4" s="0"/>
-      <c r="AMG4" s="0"/>
-      <c r="AMH4" s="0"/>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
+      <c r="ALI4" s="8"/>
+      <c r="ALJ4" s="8"/>
+      <c r="ALK4" s="8"/>
+      <c r="ALL4" s="8"/>
+      <c r="ALM4" s="8"/>
+      <c r="ALN4" s="8"/>
+      <c r="ALO4" s="8"/>
+      <c r="ALP4" s="8"/>
+      <c r="ALQ4" s="8"/>
+      <c r="ALR4" s="8"/>
+      <c r="ALS4" s="8"/>
+      <c r="ALT4" s="8"/>
+      <c r="ALU4" s="8"/>
+      <c r="ALV4" s="8"/>
+      <c r="ALW4" s="8"/>
+      <c r="ALX4" s="8"/>
+      <c r="ALY4" s="8"/>
+      <c r="ALZ4" s="8"/>
+      <c r="AMA4" s="8"/>
+      <c r="AMB4" s="8"/>
+      <c r="AMC4" s="8"/>
+      <c r="AMD4" s="8"/>
+      <c r="AME4" s="8"/>
+      <c r="AMF4" s="8"/>
+      <c r="AMG4" s="8"/>
+      <c r="AMH4" s="8"/>
+      <c r="AMI4" s="8"/>
+      <c r="AMJ4" s="8"/>
     </row>
-    <row r="5" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="33" t="s">
+    <row r="5" s="29" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="R5" s="33" t="e">
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
+      <c r="R5" s="29" t="e">
         <f aca="false">O5+#REF!+Q5+#REF!</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="X5" s="33" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="X5" s="29" t="e">
         <f aca="false">SUM(U5,#REF!,W5,#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="ALI5" s="0"/>
-      <c r="ALJ5" s="0"/>
-      <c r="ALK5" s="0"/>
-      <c r="ALL5" s="0"/>
-      <c r="ALM5" s="0"/>
-      <c r="ALN5" s="0"/>
-      <c r="ALO5" s="0"/>
-      <c r="ALP5" s="0"/>
-      <c r="ALQ5" s="0"/>
-      <c r="ALR5" s="0"/>
-      <c r="ALS5" s="0"/>
-      <c r="ALT5" s="0"/>
-      <c r="ALU5" s="0"/>
-      <c r="ALV5" s="0"/>
-      <c r="ALW5" s="0"/>
-      <c r="ALX5" s="0"/>
-      <c r="ALY5" s="0"/>
-      <c r="ALZ5" s="0"/>
-      <c r="AMA5" s="0"/>
-      <c r="AMB5" s="0"/>
-      <c r="AMC5" s="0"/>
-      <c r="AMD5" s="0"/>
-      <c r="AME5" s="0"/>
-      <c r="AMF5" s="0"/>
-      <c r="AMG5" s="0"/>
-      <c r="AMH5" s="0"/>
-      <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
+      <c r="ALI5" s="8"/>
+      <c r="ALJ5" s="8"/>
+      <c r="ALK5" s="8"/>
+      <c r="ALL5" s="8"/>
+      <c r="ALM5" s="8"/>
+      <c r="ALN5" s="8"/>
+      <c r="ALO5" s="8"/>
+      <c r="ALP5" s="8"/>
+      <c r="ALQ5" s="8"/>
+      <c r="ALR5" s="8"/>
+      <c r="ALS5" s="8"/>
+      <c r="ALT5" s="8"/>
+      <c r="ALU5" s="8"/>
+      <c r="ALV5" s="8"/>
+      <c r="ALW5" s="8"/>
+      <c r="ALX5" s="8"/>
+      <c r="ALY5" s="8"/>
+      <c r="ALZ5" s="8"/>
+      <c r="AMA5" s="8"/>
+      <c r="AMB5" s="8"/>
+      <c r="AMC5" s="8"/>
+      <c r="AMD5" s="8"/>
+      <c r="AME5" s="8"/>
+      <c r="AMF5" s="8"/>
+      <c r="AMG5" s="8"/>
+      <c r="AMH5" s="8"/>
+      <c r="AMI5" s="8"/>
+      <c r="AMJ5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -1033,16 +1017,16 @@
       <c r="G6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" s="5" t="s">
+      <c r="I6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="6" t="n">
+      <c r="K6" s="5" t="n">
         <v>2</v>
       </c>
       <c r="L6" s="23" t="n">
@@ -1055,13 +1039,13 @@
       <c r="N6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="7" t="n">
+      <c r="O6" s="6" t="n">
         <v>2</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q6" s="7" t="n">
+      <c r="Q6" s="6" t="n">
         <v>3</v>
       </c>
       <c r="R6" s="24" t="n">
@@ -1074,13 +1058,13 @@
       <c r="T6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="8" t="n">
+      <c r="U6" s="7" t="n">
         <v>2</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="W6" s="8" t="n">
+      <c r="W6" s="7" t="n">
         <v>2</v>
       </c>
       <c r="X6" s="25" t="n">
@@ -1088,7 +1072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -1110,16 +1094,16 @@
       <c r="G7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="6" t="n">
+      <c r="I7" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="6" t="n">
+      <c r="K7" s="5" t="n">
         <v>2</v>
       </c>
       <c r="L7" s="23" t="n">
@@ -1132,13 +1116,13 @@
       <c r="N7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="7" t="n">
+      <c r="O7" s="6" t="n">
         <v>2</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q7" s="7" t="n">
+      <c r="Q7" s="6" t="n">
         <v>3</v>
       </c>
       <c r="R7" s="24" t="n">
@@ -1151,13 +1135,13 @@
       <c r="T7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U7" s="8" t="n">
+      <c r="U7" s="7" t="n">
         <v>3</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="W7" s="8" t="n">
+      <c r="W7" s="7" t="n">
         <v>2</v>
       </c>
       <c r="X7" s="25" t="n">
@@ -1165,7 +1149,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
@@ -1187,16 +1171,16 @@
       <c r="G8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="I8" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="6" t="n">
+      <c r="K8" s="5" t="n">
         <v>2</v>
       </c>
       <c r="L8" s="23" t="n">
@@ -1209,13 +1193,13 @@
       <c r="N8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="7" t="n">
+      <c r="O8" s="6" t="n">
         <v>3</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q8" s="7" t="n">
+      <c r="Q8" s="6" t="n">
         <v>3</v>
       </c>
       <c r="R8" s="24" t="n">
@@ -1228,13 +1212,13 @@
       <c r="T8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="U8" s="8" t="n">
+      <c r="U8" s="7" t="n">
         <v>2</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="W8" s="8" t="n">
+      <c r="W8" s="7" t="n">
         <v>2</v>
       </c>
       <c r="X8" s="25" t="n">
@@ -1242,59 +1226,57 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="33" t="s">
+    <row r="9" s="29" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="R9" s="33" t="e">
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="R9" s="29" t="e">
         <f aca="false">O9+#REF!+Q9+#REF!</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="X9" s="33" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="X9" s="29" t="e">
         <f aca="false">SUM(U9,#REF!,W9,#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="ALI9" s="0"/>
-      <c r="ALJ9" s="0"/>
-      <c r="ALK9" s="0"/>
-      <c r="ALL9" s="0"/>
-      <c r="ALM9" s="0"/>
-      <c r="ALN9" s="0"/>
-      <c r="ALO9" s="0"/>
-      <c r="ALP9" s="0"/>
-      <c r="ALQ9" s="0"/>
-      <c r="ALR9" s="0"/>
-      <c r="ALS9" s="0"/>
-      <c r="ALT9" s="0"/>
-      <c r="ALU9" s="0"/>
-      <c r="ALV9" s="0"/>
-      <c r="ALW9" s="0"/>
-      <c r="ALX9" s="0"/>
-      <c r="ALY9" s="0"/>
-      <c r="ALZ9" s="0"/>
-      <c r="AMA9" s="0"/>
-      <c r="AMB9" s="0"/>
-      <c r="AMC9" s="0"/>
-      <c r="AMD9" s="0"/>
-      <c r="AME9" s="0"/>
-      <c r="AMF9" s="0"/>
-      <c r="AMG9" s="0"/>
-      <c r="AMH9" s="0"/>
-      <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
+      <c r="ALI9" s="8"/>
+      <c r="ALJ9" s="8"/>
+      <c r="ALK9" s="8"/>
+      <c r="ALL9" s="8"/>
+      <c r="ALM9" s="8"/>
+      <c r="ALN9" s="8"/>
+      <c r="ALO9" s="8"/>
+      <c r="ALP9" s="8"/>
+      <c r="ALQ9" s="8"/>
+      <c r="ALR9" s="8"/>
+      <c r="ALS9" s="8"/>
+      <c r="ALT9" s="8"/>
+      <c r="ALU9" s="8"/>
+      <c r="ALV9" s="8"/>
+      <c r="ALW9" s="8"/>
+      <c r="ALX9" s="8"/>
+      <c r="ALY9" s="8"/>
+      <c r="ALZ9" s="8"/>
+      <c r="AMA9" s="8"/>
+      <c r="AMB9" s="8"/>
+      <c r="AMC9" s="8"/>
+      <c r="AMD9" s="8"/>
+      <c r="AME9" s="8"/>
+      <c r="AMF9" s="8"/>
+      <c r="AMG9" s="8"/>
+      <c r="AMH9" s="8"/>
+      <c r="AMI9" s="8"/>
+      <c r="AMJ9" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="37"/>
+      <c r="C13" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="37"/>
+      <c r="C24" s="32"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="37"/>
+      <c r="C27" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>